<commit_message>
talleres 26 agosto 2024
</commit_message>
<xml_diff>
--- a/excel/Copia de ejercicio con referencias mixtas banca 2-4(1).xlsx
+++ b/excel/Copia de ejercicio con referencias mixtas banca 2-4(1).xlsx
@@ -1413,6 +1413,8 @@
     <xf numFmtId="1" fontId="16" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1464,8 +1466,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1492,15 +1492,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1511,8 +1511,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5276850" y="1552575"/>
-          <a:ext cx="2438400" cy="1343025"/>
+          <a:off x="4238625" y="2133600"/>
+          <a:ext cx="2438400" cy="1581150"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
           <a:avLst>
@@ -1590,14 +1590,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -1610,8 +1610,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5286375" y="161925"/>
-          <a:ext cx="2438400" cy="1333500"/>
+          <a:off x="4619625" y="190500"/>
+          <a:ext cx="2438400" cy="1600200"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
           <a:avLst>
@@ -1619,8 +1619,8 @@
             <a:gd name="adj2" fmla="val -3125"/>
             <a:gd name="adj3" fmla="val 8569"/>
             <a:gd name="adj4" fmla="val -16014"/>
-            <a:gd name="adj5" fmla="val 57856"/>
-            <a:gd name="adj6" fmla="val -26171"/>
+            <a:gd name="adj5" fmla="val 51904"/>
+            <a:gd name="adj6" fmla="val -35155"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -1709,7 +1709,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="762000" y="2781300"/>
+          <a:off x="762000" y="2828925"/>
           <a:ext cx="1447800" cy="828675"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
@@ -1718,8 +1718,8 @@
             <a:gd name="adj2" fmla="val 105194"/>
             <a:gd name="adj3" fmla="val 16000"/>
             <a:gd name="adj4" fmla="val 126625"/>
-            <a:gd name="adj5" fmla="val -16000"/>
-            <a:gd name="adj6" fmla="val 144157"/>
+            <a:gd name="adj5" fmla="val -14851"/>
+            <a:gd name="adj6" fmla="val 123104"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -2129,14 +2129,14 @@
       <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="96" t="s">
+      <c r="J2" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="2:15">
       <c r="B3" t="s">
@@ -2152,7 +2152,7 @@
         <f>+D3*C16</f>
         <v>3000</v>
       </c>
-      <c r="F3" s="113">
+      <c r="F3" s="96">
         <f>+E3*F$16</f>
         <v>60</v>
       </c>
@@ -2168,12 +2168,12 @@
         <f>+G3+H3</f>
         <v>3410.4</v>
       </c>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -2189,7 +2189,7 @@
         <f>+D4*C17</f>
         <v>12000</v>
       </c>
-      <c r="F4" s="113">
+      <c r="F4" s="96">
         <f t="shared" ref="F4:F8" si="0">+E4*F$16</f>
         <v>240</v>
       </c>
@@ -2205,12 +2205,12 @@
         <f>+G4+H4</f>
         <v>13641.6</v>
       </c>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="96"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="98"/>
     </row>
     <row r="5" spans="2:15">
       <c r="C5" t="s">
@@ -2223,7 +2223,7 @@
         <f>+D5*C18</f>
         <v>5000</v>
       </c>
-      <c r="F5" s="113">
+      <c r="F5" s="96">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -2239,12 +2239,12 @@
         <f>+G5+H5</f>
         <v>5684</v>
       </c>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
     </row>
     <row r="6" spans="2:15">
       <c r="C6" t="s">
@@ -2254,10 +2254,10 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E4:E8" si="2">+D6*C19</f>
+        <f t="shared" ref="E6:E7" si="2">+D6*C19</f>
         <v>64000</v>
       </c>
-      <c r="F6" s="113">
+      <c r="F6" s="96">
         <f t="shared" si="0"/>
         <v>1280</v>
       </c>
@@ -2266,19 +2266,19 @@
         <v>62720</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H4:H8" si="3">+G6*F$17</f>
+        <f t="shared" ref="H6:H8" si="3">+G6*F$17</f>
         <v>10035.200000000001</v>
       </c>
       <c r="I6">
         <f>+G6+H6</f>
         <v>72755.199999999997</v>
       </c>
-      <c r="J6" s="96"/>
-      <c r="K6" s="96"/>
-      <c r="L6" s="96"/>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="98"/>
     </row>
     <row r="7" spans="2:15">
       <c r="C7" t="s">
@@ -2291,7 +2291,7 @@
         <f t="shared" si="2"/>
         <v>45000</v>
       </c>
-      <c r="F7" s="113">
+      <c r="F7" s="96">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
@@ -2304,15 +2304,15 @@
         <v>7056</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I4:I8" si="4">+G7+H7</f>
+        <f t="shared" ref="I7:I8" si="4">+G7+H7</f>
         <v>51156</v>
       </c>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="96"/>
-      <c r="O7" s="96"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
     </row>
     <row r="8" spans="2:15">
       <c r="C8" t="s">
@@ -2325,7 +2325,7 @@
         <f>+D8*C21</f>
         <v>51200</v>
       </c>
-      <c r="F8" s="113">
+      <c r="F8" s="96">
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
@@ -2341,60 +2341,60 @@
         <f t="shared" si="4"/>
         <v>58204.160000000003</v>
       </c>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="96"/>
-      <c r="O8" s="96"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
     </row>
     <row r="9" spans="2:15">
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
-      <c r="N9" s="96"/>
-      <c r="O9" s="96"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="98"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
-      <c r="N10" s="96"/>
-      <c r="O10" s="96"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
+      <c r="O10" s="98"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="J11" s="96"/>
-      <c r="K11" s="96"/>
-      <c r="L11" s="96"/>
-      <c r="M11" s="96"/>
-      <c r="N11" s="96"/>
-      <c r="O11" s="96"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="98"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="J12" s="96"/>
-      <c r="K12" s="96"/>
-      <c r="L12" s="96"/>
-      <c r="M12" s="96"/>
-      <c r="N12" s="96"/>
-      <c r="O12" s="96"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="J13" s="96"/>
-      <c r="K13" s="96"/>
-      <c r="L13" s="96"/>
-      <c r="M13" s="96"/>
-      <c r="N13" s="96"/>
-      <c r="O13" s="96"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="J14" s="96"/>
-      <c r="K14" s="96"/>
-      <c r="L14" s="96"/>
-      <c r="M14" s="96"/>
-      <c r="N14" s="96"/>
-      <c r="O14" s="96"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
+      <c r="O14" s="98"/>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
@@ -2403,12 +2403,12 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="96"/>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="96"/>
-      <c r="O15" s="96"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
@@ -2423,12 +2423,12 @@
       <c r="F16" s="1">
         <v>0.02</v>
       </c>
-      <c r="J16" s="96"/>
-      <c r="K16" s="96"/>
-      <c r="L16" s="96"/>
-      <c r="M16" s="96"/>
-      <c r="N16" s="96"/>
-      <c r="O16" s="96"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="98"/>
     </row>
     <row r="17" spans="2:15">
       <c r="B17" t="s">
@@ -2443,12 +2443,12 @@
       <c r="F17" s="1">
         <v>0.16</v>
       </c>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="98"/>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" t="s">
@@ -2457,12 +2457,12 @@
       <c r="C18">
         <v>5000</v>
       </c>
-      <c r="J18" s="96"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="96"/>
-      <c r="M18" s="96"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="96"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="98"/>
     </row>
     <row r="19" spans="2:15">
       <c r="B19" t="s">
@@ -2471,12 +2471,12 @@
       <c r="C19">
         <v>8000</v>
       </c>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="96"/>
-      <c r="M19" s="96"/>
-      <c r="N19" s="96"/>
-      <c r="O19" s="96"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="98"/>
     </row>
     <row r="20" spans="2:15">
       <c r="B20" t="s">
@@ -2485,12 +2485,12 @@
       <c r="C20">
         <v>4500</v>
       </c>
-      <c r="J20" s="96"/>
-      <c r="K20" s="96"/>
-      <c r="L20" s="96"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="96"/>
-      <c r="O20" s="96"/>
+      <c r="J20" s="98"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="98"/>
+      <c r="O20" s="98"/>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
@@ -2499,12 +2499,12 @@
       <c r="C21">
         <v>3200</v>
       </c>
-      <c r="J21" s="96"/>
-      <c r="K21" s="96"/>
-      <c r="L21" s="96"/>
-      <c r="M21" s="96"/>
-      <c r="N21" s="96"/>
-      <c r="O21" s="96"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2532,17 +2532,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
     </row>
     <row r="2" spans="2:13">
       <c r="E2" s="1">
@@ -2582,91 +2582,91 @@
       <c r="C4" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="114">
+      <c r="D4" s="97">
         <v>120000000</v>
       </c>
-      <c r="E4" s="114">
+      <c r="E4" s="97">
         <f>+D4*E$2</f>
         <v>24000000</v>
       </c>
-      <c r="F4" s="114">
+      <c r="F4" s="97">
         <v>70000000</v>
       </c>
-      <c r="G4" s="114">
+      <c r="G4" s="97">
         <f>+D4-E4-F4</f>
         <v>26000000</v>
       </c>
-      <c r="I4" s="97" t="s">
+      <c r="I4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
     </row>
     <row r="5" spans="2:13">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="G5" s="3"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="99"/>
     </row>
     <row r="6" spans="2:13">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="97"/>
-      <c r="M6" s="97"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
     </row>
     <row r="7" spans="2:13">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="97"/>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="97"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="99"/>
     </row>
     <row r="8" spans="2:13">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="I8" s="97"/>
-      <c r="J8" s="97"/>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="99"/>
     </row>
     <row r="9" spans="2:13">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="97"/>
-      <c r="K9" s="97"/>
-      <c r="L9" s="97"/>
-      <c r="M9" s="97"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="99"/>
     </row>
     <row r="10" spans="2:13">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="97"/>
-      <c r="L10" s="97"/>
-      <c r="M10" s="97"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="99"/>
     </row>
     <row r="11" spans="2:13">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="I11" s="97"/>
-      <c r="J11" s="97"/>
-      <c r="K11" s="97"/>
-      <c r="L11" s="97"/>
-      <c r="M11" s="97"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="99"/>
+      <c r="M11" s="99"/>
     </row>
     <row r="12" spans="2:13">
       <c r="D12" s="2"/>
@@ -2707,10 +2707,13 @@
   <dimension ref="A3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D6:J12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:5">
       <c r="D3" s="4" t="s">
@@ -2756,12 +2759,12 @@
         <v>18</v>
       </c>
       <c r="D6" s="10">
-        <f>+B6*C6-D$4</f>
-        <v>179.9</v>
+        <f>+(B6*C6)-(B6*C6*D$4)</f>
+        <v>162</v>
       </c>
       <c r="E6" s="11">
-        <f>+B6*C6+E$4</f>
-        <v>180.2</v>
+        <f>+(B6*C6)+(B6*C6*E$4)</f>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1">
@@ -2775,12 +2778,12 @@
         <v>19</v>
       </c>
       <c r="D7" s="10">
-        <f t="shared" ref="D7:D11" si="0">+B7*C7-D$4</f>
-        <v>398.9</v>
+        <f>+(B7*C7)-(B7*C7*D$4)</f>
+        <v>359.1</v>
       </c>
       <c r="E7" s="11">
-        <f>+B7*C7+E$4</f>
-        <v>399.2</v>
+        <f t="shared" ref="E7:E11" si="0">+(B7*C7)+(B7*C7*E$4)</f>
+        <v>478.8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
@@ -2794,12 +2797,12 @@
         <v>10</v>
       </c>
       <c r="D8" s="10">
+        <f t="shared" ref="D7:D11" si="1">+(B8*C8)-(B8*C8*D$4)</f>
+        <v>396</v>
+      </c>
+      <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>439.9</v>
-      </c>
-      <c r="E8" s="11">
-        <f>+B8*C8+E$4</f>
-        <v>440.2</v>
+        <v>528</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1">
@@ -2813,12 +2816,12 @@
         <v>22</v>
       </c>
       <c r="D9" s="10">
+        <f t="shared" si="1"/>
+        <v>435.6</v>
+      </c>
+      <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>483.9</v>
-      </c>
-      <c r="E9" s="11">
-        <f t="shared" ref="E7:E11" si="1">+B9*C9+E$4</f>
-        <v>484.2</v>
+        <v>580.79999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1">
@@ -2832,12 +2835,12 @@
         <v>21.35</v>
       </c>
       <c r="D10" s="10">
+        <f t="shared" si="1"/>
+        <v>614.88</v>
+      </c>
+      <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>683.1</v>
-      </c>
-      <c r="E10" s="11">
-        <f t="shared" si="1"/>
-        <v>683.40000000000009</v>
+        <v>819.84</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1">
@@ -2851,12 +2854,12 @@
         <v>25</v>
       </c>
       <c r="D11" s="10">
+        <f>+(B11*C11)-(B11*C11*D$4)</f>
+        <v>270</v>
+      </c>
+      <c r="E11" s="11">
         <f t="shared" si="0"/>
-        <v>299.89999999999998</v>
-      </c>
-      <c r="E11" s="11">
-        <f t="shared" si="1"/>
-        <v>300.2</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1">
@@ -2865,7 +2868,10 @@
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
+      <c r="D12" s="16">
+        <f>SUM(D6:D11)</f>
+        <v>2237.58</v>
+      </c>
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1">
@@ -2875,7 +2881,10 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="16"/>
+      <c r="E13" s="16">
+        <f>SUM(E6:E11)</f>
+        <v>2983.44</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1">
       <c r="A14" s="14" t="s">
@@ -2883,7 +2892,10 @@
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="D14" s="16">
+        <f>E13-D12</f>
+        <v>745.86000000000013</v>
+      </c>
       <c r="E14" s="17"/>
     </row>
   </sheetData>
@@ -2904,16 +2916,16 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="101"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="103"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1">
       <c r="B4" s="18"/>
@@ -3209,14 +3221,14 @@
       <c r="D3" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="104" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
     </row>
     <row r="4" spans="3:10">
       <c r="E4">
@@ -3334,15 +3346,15 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1">
-      <c r="E3" s="103" t="s">
+      <c r="E3" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="B4" s="35" t="s">
@@ -3821,27 +3833,27 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="106" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
       <c r="F1" s="56"/>
       <c r="G1" s="56"/>
       <c r="H1" s="56"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="106"/>
+      <c r="B2" s="108"/>
       <c r="C2" s="57"/>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="109" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="108"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="57"/>
       <c r="G2" s="58"/>
       <c r="H2" s="58"/>
@@ -4204,19 +4216,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="22.5">
-      <c r="B1" s="109" t="s">
+      <c r="B1" s="111" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="81" t="s">
@@ -4248,21 +4260,21 @@
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1"/>
     <row r="5" spans="2:12" ht="16.5" thickBot="1">
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="112" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="111"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="110" t="s">
+      <c r="D5" s="113"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="112" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="111"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="110" t="s">
+      <c r="G5" s="113"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="112" t="s">
         <v>136</v>
       </c>
-      <c r="J5" s="111"/>
-      <c r="K5" s="112"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="114"/>
     </row>
     <row r="6" spans="2:12" ht="18.75">
       <c r="B6" s="83" t="s">

</xml_diff>